<commit_message>
able to add series systems from excel file, need to add parallel system functionality
</commit_message>
<xml_diff>
--- a/shipClassTests/AuxilaryPropulsionPlant_Reliability_Availability_Data.xlsx
+++ b/shipClassTests/AuxilaryPropulsionPlant_Reliability_Availability_Data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andreya.Ware.ctr\Desktop\KISS_NSWCPD_Copy\KISS\shipClassTests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adware\Desktop\KISS\shipClassTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106C01CC-F644-455F-8786-2C731EFCCD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F776CDA1-903E-4A1A-96CE-614223088FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-7440" windowWidth="16440" windowHeight="28320" xr2:uid="{279480E9-DBDF-4252-B432-4CE1D30BF378}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{279480E9-DBDF-4252-B432-4CE1D30BF378}"/>
   </bookViews>
   <sheets>
     <sheet name="machinery reliability data" sheetId="1" r:id="rId1"/>
+    <sheet name="system structure data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Component</t>
   </si>
@@ -93,6 +94,30 @@
   </si>
   <si>
     <t>NR</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>diesel engine system</t>
+  </si>
+  <si>
+    <t>transmission system</t>
+  </si>
+  <si>
+    <t>[8, 9, 10, 11, 12, 6, 0, 1]</t>
+  </si>
+  <si>
+    <t>[ 2, 3, 4]</t>
+  </si>
+  <si>
+    <t>fuel oil system</t>
+  </si>
+  <si>
+    <t>[([5,6], [5,6]), (7,7)]</t>
   </si>
 </sst>
 </file>
@@ -489,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F997A0B-9C86-4EC5-9A0F-10545207BFB0}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -742,4 +767,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4FF0A7-4C32-4212-8D10-DADC32F7B7B8}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="32.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed ship initialization from excel file, working on sys diagrams
</commit_message>
<xml_diff>
--- a/shipClassTests/AuxilaryPropulsionPlant_Reliability_Availability_Data.xlsx
+++ b/shipClassTests/AuxilaryPropulsionPlant_Reliability_Availability_Data.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adware\Desktop\KISS\shipClassTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F776CDA1-903E-4A1A-96CE-614223088FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB07C6DA-609E-4B59-A987-F5F229D17122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{279480E9-DBDF-4252-B432-4CE1D30BF378}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{279480E9-DBDF-4252-B432-4CE1D30BF378}"/>
   </bookViews>
   <sheets>
     <sheet name="machinery reliability data" sheetId="1" r:id="rId1"/>
     <sheet name="system structure data" sheetId="2" r:id="rId2"/>
+    <sheet name="notes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Component</t>
   </si>
@@ -114,7 +115,16 @@
     <t>[ 2, 3, 4]</t>
   </si>
   <si>
-    <t>fuel oil system</t>
+    <t>test system</t>
+  </si>
+  <si>
+    <t>python idx</t>
+  </si>
+  <si>
+    <t>[(9,9), 4]</t>
+  </si>
+  <si>
+    <t>fuel system</t>
   </si>
   <si>
     <t>[([5,6], [5,6]), (7,7)]</t>
@@ -173,10 +183,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -512,254 +525,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F997A0B-9C86-4EC5-9A0F-10545207BFB0}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="A1:XFD1048576"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="2" customWidth="1"/>
-    <col min="3" max="5" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="2" customWidth="1"/>
+    <col min="4" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="C2" s="2">
         <v>8000</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>0.999</v>
-      </c>
       <c r="E2">
         <v>0.999</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="2">
         <v>50000</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.98599999999999999</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="2">
         <v>200000</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.996</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="2">
         <v>200000</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.996</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="2">
         <v>25000</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>15</v>
       </c>
-      <c r="D6">
-        <v>0.999</v>
-      </c>
       <c r="E6">
         <v>0.999</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C7" s="2">
         <v>7500</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>18</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.998</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>0.997</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="2">
         <v>5500</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>4.5</v>
       </c>
-      <c r="D8">
-        <v>0.999</v>
-      </c>
       <c r="E8">
         <v>0.999</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F8">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C9" s="2">
         <v>10000</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>4</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="E9">
-        <v>0.999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C10" s="2">
         <v>7500</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>7.8</v>
       </c>
-      <c r="D10">
-        <v>0.999</v>
-      </c>
       <c r="E10">
+        <v>0.999</v>
+      </c>
+      <c r="F10">
         <v>0.998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2">
+      <c r="C11" s="2">
         <v>4000</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>5</v>
       </c>
-      <c r="D11">
-        <v>0.999</v>
-      </c>
       <c r="E11">
+        <v>0.999</v>
+      </c>
+      <c r="F11">
         <v>0.998</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="2">
+      <c r="C12" s="2">
         <v>27000</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>7.6</v>
       </c>
-      <c r="D12">
-        <v>0.999</v>
-      </c>
       <c r="E12">
         <v>0.999</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F12">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2">
+      <c r="C13" s="2">
         <v>12500</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>12</v>
       </c>
-      <c r="D13">
-        <v>0.999</v>
-      </c>
       <c r="E13">
         <v>0.999</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="F13">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2">
+      <c r="C14" s="2">
         <v>5500</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>4.5</v>
       </c>
-      <c r="D14">
-        <v>0.999</v>
-      </c>
       <c r="E14">
+        <v>0.999</v>
+      </c>
+      <c r="F14">
         <v>0.999</v>
       </c>
     </row>
@@ -771,10 +827,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4FF0A7-4C32-4212-8D10-DADC32F7B7B8}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,30 +848,65 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B338D18E-1C2C-4003-BC79-5462DE0704E2}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed ship initalization from excel file
</commit_message>
<xml_diff>
--- a/shipClassTests/AuxilaryPropulsionPlant_Reliability_Availability_Data.xlsx
+++ b/shipClassTests/AuxilaryPropulsionPlant_Reliability_Availability_Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adware\Desktop\KISS\shipClassTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB07C6DA-609E-4B59-A987-F5F229D17122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21280CAC-8E2B-4B3E-8430-B7D5C43E0FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{279480E9-DBDF-4252-B432-4CE1D30BF378}"/>
+    <workbookView xWindow="11100" yWindow="5820" windowWidth="11535" windowHeight="8550" firstSheet="1" activeTab="1" xr2:uid="{279480E9-DBDF-4252-B432-4CE1D30BF378}"/>
   </bookViews>
   <sheets>
     <sheet name="machinery reliability data" sheetId="1" r:id="rId1"/>
     <sheet name="system structure data" sheetId="2" r:id="rId2"/>
-    <sheet name="notes" sheetId="3" r:id="rId3"/>
+    <sheet name="ship structure" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>Component</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Shaft and Bearings</t>
   </si>
   <si>
-    <t>CRP Propellers</t>
-  </si>
-  <si>
     <t>Fuel Oil Motor</t>
   </si>
   <si>
@@ -103,31 +100,37 @@
     <t>Structure</t>
   </si>
   <si>
-    <t>diesel engine system</t>
+    <t>python idx</t>
+  </si>
+  <si>
+    <t>ship structure</t>
+  </si>
+  <si>
+    <t>Sys Index</t>
+  </si>
+  <si>
+    <t>[0,1,2,3]</t>
   </si>
   <si>
     <t>transmission system</t>
   </si>
   <si>
+    <t>[2,3,4]</t>
+  </si>
+  <si>
+    <t>CRP Propeller</t>
+  </si>
+  <si>
+    <t>fuel system</t>
+  </si>
+  <si>
     <t>[8, 9, 10, 11, 12, 6, 0, 1]</t>
   </si>
   <si>
-    <t>[ 2, 3, 4]</t>
-  </si>
-  <si>
-    <t>test system</t>
-  </si>
-  <si>
-    <t>python idx</t>
-  </si>
-  <si>
-    <t>[(9,9), 4]</t>
-  </si>
-  <si>
-    <t>fuel system</t>
-  </si>
-  <si>
-    <t>[([5,6], [5,6]), (7,7)]</t>
+    <t xml:space="preserve">diesel engine system </t>
+  </si>
+  <si>
+    <t>[([5,6], [5,6]), (7,7) ]</t>
   </si>
 </sst>
 </file>
@@ -138,7 +141,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +158,14 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -183,13 +194,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -525,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F997A0B-9C86-4EC5-9A0F-10545207BFB0}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +554,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -590,7 +603,7 @@
         <v>50000</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>0.98599999999999999</v>
@@ -610,7 +623,7 @@
         <v>200000</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4">
         <v>0.996</v>
@@ -630,7 +643,7 @@
         <v>200000</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5">
         <v>0.996</v>
@@ -644,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>25000</v>
@@ -664,7 +677,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2">
         <v>7500</v>
@@ -684,7 +697,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2">
         <v>5500</v>
@@ -704,7 +717,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2">
         <v>10000</v>
@@ -724,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2">
         <v>7500</v>
@@ -744,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2">
         <v>4000</v>
@@ -764,7 +777,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" s="2">
         <v>27000</v>
@@ -784,7 +797,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="2">
         <v>12500</v>
@@ -804,7 +817,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2">
         <v>5500</v>
@@ -818,6 +831,9 @@
       <c r="F14">
         <v>0.999</v>
       </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -827,32 +843,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4FF0A7-4C32-4212-8D10-DADC32F7B7B8}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="32.42578125" customWidth="1"/>
+    <col min="2" max="3" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -862,10 +909,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B338D18E-1C2C-4003-BC79-5462DE0704E2}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,33 +923,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated sensed systems and ships; adding Q1 simulator
</commit_message>
<xml_diff>
--- a/shipClassTests/AuxilaryPropulsionPlant_Reliability_Availability_Data.xlsx
+++ b/shipClassTests/AuxilaryPropulsionPlant_Reliability_Availability_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adware\Desktop\KISS\shipClassTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21280CAC-8E2B-4B3E-8430-B7D5C43E0FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EEB61F-4014-45B0-93B9-2A1EFBA389D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11100" yWindow="5820" windowWidth="11535" windowHeight="8550" firstSheet="1" activeTab="1" xr2:uid="{279480E9-DBDF-4252-B432-4CE1D30BF378}"/>
+    <workbookView xWindow="11100" yWindow="5820" windowWidth="11535" windowHeight="8550" firstSheet="2" activeTab="2" xr2:uid="{279480E9-DBDF-4252-B432-4CE1D30BF378}"/>
   </bookViews>
   <sheets>
     <sheet name="machinery reliability data" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Sys Index</t>
   </si>
   <si>
-    <t>[0,1,2,3]</t>
-  </si>
-  <si>
     <t>transmission system</t>
   </si>
   <si>
@@ -131,6 +128,9 @@
   </si>
   <si>
     <t>[([5,6], [5,6]), (7,7) ]</t>
+  </si>
+  <si>
+    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -657,7 +657,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2">
         <v>25000</v>
@@ -845,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4FF0A7-4C32-4212-8D10-DADC32F7B7B8}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -870,10 +870,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -881,10 +881,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -892,10 +892,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -911,7 +911,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B338D18E-1C2C-4003-BC79-5462DE0704E2}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -929,7 +929,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>